<commit_message>
//fixes in gw and cvhan wf flow
</commit_message>
<xml_diff>
--- a/auxfiles/GSSHApedotransfer.xlsx
+++ b/auxfiles/GSSHApedotransfer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302015E4-826E-4262-9429-1906896561C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC4FE7D-B358-43EF-BA8F-3D0F31B8F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{EE7E3014-B43F-4E75-BCA9-657834F4F7BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EE7E3014-B43F-4E75-BCA9-657834F4F7BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,7 +331,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -483,9 +483,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -496,11 +493,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -560,7 +560,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -640,7 +640,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -803,7 +803,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1958513087"/>
@@ -865,7 +865,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1958512127"/>
@@ -913,7 +913,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -964,7 +964,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1044,7 +1044,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1207,7 +1207,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="825484127"/>
@@ -1269,7 +1269,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="825487487"/>
@@ -1317,7 +1317,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1368,7 +1368,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1448,7 +1448,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1610,7 +1610,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="918899471"/>
@@ -1672,7 +1672,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="918901871"/>
@@ -1720,7 +1720,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1771,7 +1771,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1851,7 +1851,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2013,7 +2013,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="349209424"/>
@@ -2075,7 +2075,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="349207504"/>
@@ -2123,7 +2123,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2203,7 +2203,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2293,7 +2293,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2472,7 +2472,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2510,7 +2510,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="349205312"/>
@@ -2598,7 +2598,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2636,7 +2636,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="349202912"/>
@@ -2684,7 +2684,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2768,7 +2768,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2848,7 +2848,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3010,7 +3010,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="348374448"/>
@@ -3072,7 +3072,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="348376368"/>
@@ -3120,7 +3120,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3171,7 +3171,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3251,7 +3251,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3413,7 +3413,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="293480000"/>
@@ -3475,7 +3475,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="293478560"/>
@@ -3523,7 +3523,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3607,7 +3607,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3687,7 +3687,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -3849,7 +3849,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564138272"/>
@@ -3911,7 +3911,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="564140672"/>
@@ -3959,7 +3959,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4035,7 +4035,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="nl-NL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4125,7 +4125,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="nl-NL"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4287,7 +4287,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="556251872"/>
@@ -4349,7 +4349,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1564086688"/>
@@ -4397,7 +4397,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -9648,16 +9648,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>881062</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>74295</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>50482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>319087</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>379095</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>75247</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9720,16 +9720,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>576263</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>530543</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>271463</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>225743</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>77151</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9829,15 +9829,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>340521</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
+      <xdr:colOff>584361</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>267653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>35721</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>290513</xdr:rowOff>
+      <xdr:colOff>279561</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>168593</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10164,31 +10164,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC7A993-96B8-4AA6-8EF4-C236C394CA84}">
   <dimension ref="F1:AA18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="J6" workbookViewId="0">
+      <selection activeCell="W8" sqref="W8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="F1" s="5" t="s">
+    <row r="1" spans="6:27" x14ac:dyDescent="0.3">
+      <c r="F1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
-    <row r="3" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="F3" s="6" t="s">
+    <row r="3" spans="6:27" x14ac:dyDescent="0.3">
+      <c r="F3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="6:27" ht="165" x14ac:dyDescent="0.25">
-      <c r="F4" s="4" t="s">
+    <row r="4" spans="6:27" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="F4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
@@ -10223,8 +10223,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="6:27" ht="18" x14ac:dyDescent="0.25">
-      <c r="F5" s="4"/>
+    <row r="5" spans="6:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="F5" s="12"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2" t="s">
@@ -10255,8 +10255,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="6:27" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="F6" s="4"/>
+    <row r="6" spans="6:27" ht="45" x14ac:dyDescent="0.3">
+      <c r="F6" s="12"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2" t="s">
@@ -10305,11 +10305,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="6:27" x14ac:dyDescent="0.25">
-      <c r="G7" s="7" t="s">
+    <row r="7" spans="6:27" x14ac:dyDescent="0.3">
+      <c r="G7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>46</v>
       </c>
       <c r="S7" t="s">
@@ -10319,15 +10319,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f>P8*10</f>
         <v>235.6</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <f>LN(G8)</f>
         <v>5.4621354517774314</v>
       </c>
@@ -10383,11 +10383,11 @@
         <v>1.5993875765805989</v>
       </c>
       <c r="Y8">
-        <f>O8</f>
+        <f t="shared" ref="Y8:Y18" si="0">O8</f>
         <v>0.69399999999999995</v>
       </c>
       <c r="Z8">
-        <f>LN(S8)</f>
+        <f t="shared" ref="Z8:Z18" si="1">LN(S8)</f>
         <v>5.4621354517774314</v>
       </c>
       <c r="AA8">
@@ -10395,16 +10395,16 @@
         <v>-0.36528331847533263</v>
       </c>
     </row>
-    <row r="9" spans="6:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="9">
-        <f t="shared" ref="G9:G18" si="0">P9*10</f>
+      <c r="G9" s="8">
+        <f t="shared" ref="G9:G18" si="2">P9*10</f>
         <v>59.800000000000004</v>
       </c>
-      <c r="H9" s="11">
-        <f t="shared" ref="H9:H18" si="1">LN(G9)</f>
+      <c r="H9" s="10">
+        <f t="shared" ref="H9:H18" si="3">LN(G9)</f>
         <v>4.0910056609565864</v>
       </c>
       <c r="I9" s="2">
@@ -10435,723 +10435,723 @@
         <v>6.13</v>
       </c>
       <c r="S9">
-        <f t="shared" ref="S9:S18" si="2">P9*10</f>
+        <f t="shared" ref="S9:S18" si="4">P9*10</f>
         <v>59.800000000000004</v>
       </c>
       <c r="T9">
-        <f t="shared" ref="T9:T18" si="3">Q9</f>
+        <f t="shared" ref="T9:T18" si="5">Q9</f>
         <v>6.13</v>
       </c>
       <c r="U9">
-        <f>LOG(S9)</f>
+        <f t="shared" ref="U9:U18" si="6">LOG(S9)</f>
         <v>1.7767011839884108</v>
       </c>
       <c r="V9">
-        <f t="shared" ref="V9:V18" si="4">LOG(T9)</f>
+        <f t="shared" ref="V9:V18" si="7">LOG(T9)</f>
         <v>0.78746047451841505</v>
       </c>
       <c r="W9">
-        <f t="shared" ref="W9:W18" si="5">LN(S9)</f>
+        <f t="shared" ref="W9:W18" si="8">LN(S9)</f>
         <v>4.0910056609565864</v>
       </c>
       <c r="X9">
-        <f t="shared" ref="X9:X18" si="6">LN(T9)</f>
+        <f t="shared" ref="X9:X18" si="9">LN(T9)</f>
         <v>1.81319474994812</v>
       </c>
       <c r="Y9">
-        <f>O9</f>
+        <f t="shared" si="0"/>
         <v>0.55300000000000005</v>
       </c>
       <c r="Z9">
-        <f>LN(S9)</f>
+        <f t="shared" si="1"/>
         <v>4.0910056609565864</v>
       </c>
       <c r="AA9">
-        <f t="shared" ref="AA9:AA18" si="7">LN(Y9)</f>
+        <f t="shared" ref="AA9:AA18" si="10">LN(Y9)</f>
         <v>-0.5923972774598022</v>
       </c>
     </row>
-    <row r="10" spans="6:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
+        <f t="shared" si="2"/>
+        <v>21.8</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="3"/>
+        <v>3.0819099697950434</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="L10" s="2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="M10" s="2">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>14.66</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0.378</v>
+      </c>
+      <c r="P10" s="2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>11.01</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>21.8</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="5"/>
+        <v>11.01</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="6"/>
+        <v>1.3384564936046048</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="7"/>
+        <v>1.0417873189717517</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="8"/>
+        <v>3.0819099697950434</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="9"/>
+        <v>2.3988039507345884</v>
+      </c>
+      <c r="Y10">
         <f t="shared" si="0"/>
-        <v>21.8</v>
-      </c>
-      <c r="H10" s="11">
+        <v>0.378</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="1"/>
         <v>3.0819099697950434</v>
       </c>
-      <c r="I10" s="2">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.41199999999999998</v>
-      </c>
-      <c r="K10" s="2">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="L10" s="2">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="M10" s="2">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="N10" s="2">
-        <v>14.66</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0.378</v>
-      </c>
-      <c r="P10" s="2">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>11.01</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="2"/>
-        <v>21.8</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="3"/>
-        <v>11.01</v>
-      </c>
-      <c r="U10">
-        <f>LOG(S10)</f>
-        <v>1.3384564936046048</v>
-      </c>
-      <c r="V10">
-        <f t="shared" si="4"/>
-        <v>1.0417873189717517</v>
-      </c>
-      <c r="W10">
-        <f t="shared" si="5"/>
-        <v>3.0819099697950434</v>
-      </c>
-      <c r="X10">
-        <f t="shared" si="6"/>
-        <v>2.3988039507345884</v>
-      </c>
-      <c r="Y10">
-        <f>O10</f>
-        <v>0.378</v>
-      </c>
-      <c r="Z10">
-        <f>LN(S10)</f>
-        <v>3.0819099697950434</v>
-      </c>
       <c r="AA10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-0.97286108336254939</v>
       </c>
     </row>
-    <row r="11" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
+        <f t="shared" si="2"/>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="3"/>
+        <v>2.5802168295923251</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.434</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.27</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>2.7E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>11.15</v>
+      </c>
+      <c r="O11" s="2">
+        <v>0.252</v>
+      </c>
+      <c r="P11" s="2">
+        <v>1.32</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>8.89</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>13.200000000000001</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="5"/>
+        <v>8.89</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="6"/>
+        <v>1.1205739312058498</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="7"/>
+        <v>0.94890176097021373</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="8"/>
+        <v>2.5802168295923251</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="9"/>
+        <v>2.1849270495258133</v>
+      </c>
+      <c r="Y11">
         <f t="shared" si="0"/>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="H11" s="11">
+        <v>0.252</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="1"/>
         <v>2.5802168295923251</v>
       </c>
-      <c r="I11" s="2">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.434</v>
-      </c>
-      <c r="K11" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="M11" s="2">
-        <v>2.7E-2</v>
-      </c>
-      <c r="N11" s="2">
-        <v>11.15</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.252</v>
-      </c>
-      <c r="P11" s="2">
-        <v>1.32</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>8.89</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="2"/>
-        <v>13.200000000000001</v>
-      </c>
-      <c r="T11">
-        <f t="shared" si="3"/>
-        <v>8.89</v>
-      </c>
-      <c r="U11">
-        <f>LOG(S11)</f>
-        <v>1.1205739312058498</v>
-      </c>
-      <c r="V11">
-        <f t="shared" si="4"/>
-        <v>0.94890176097021373</v>
-      </c>
-      <c r="W11">
-        <f t="shared" si="5"/>
-        <v>2.5802168295923251</v>
-      </c>
-      <c r="X11">
-        <f t="shared" si="6"/>
-        <v>2.1849270495258133</v>
-      </c>
-      <c r="Y11">
-        <f>O11</f>
-        <v>0.252</v>
-      </c>
-      <c r="Z11">
-        <f>LN(S11)</f>
-        <v>2.5802168295923251</v>
-      </c>
       <c r="AA11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.3783261914707137</v>
       </c>
     </row>
-    <row r="12" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
+        <f t="shared" si="2"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="3"/>
+        <v>1.9169226121820611</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.501</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M12" s="2">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <v>20.79</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="P12" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>16.68</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="5"/>
+        <v>16.68</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="6"/>
+        <v>0.83250891270623639</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="7"/>
+        <v>1.2221960463017199</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="8"/>
+        <v>1.9169226121820611</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="9"/>
+        <v>2.8142103969306005</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="0"/>
-        <v>6.8000000000000007</v>
-      </c>
-      <c r="H12" s="11">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="Z12">
         <f t="shared" si="1"/>
         <v>1.9169226121820611</v>
       </c>
-      <c r="I12" s="2">
-        <v>0.501</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="L12" s="2">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N12" s="2">
-        <v>20.79</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0.68</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>16.68</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="2"/>
-        <v>6.8000000000000007</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="3"/>
-        <v>16.68</v>
-      </c>
-      <c r="U12">
-        <f>LOG(S12)</f>
-        <v>0.83250891270623639</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="4"/>
-        <v>1.2221960463017199</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="5"/>
-        <v>1.9169226121820611</v>
-      </c>
-      <c r="X12">
-        <f t="shared" si="6"/>
-        <v>2.8142103969306005</v>
-      </c>
-      <c r="Y12">
-        <f>O12</f>
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="Z12">
-        <f>LN(S12)</f>
-        <v>1.9169226121820611</v>
-      </c>
       <c r="AA12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.4524341636244356</v>
       </c>
     </row>
-    <row r="13" spans="6:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.255</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="M13" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <v>28.08</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>21.85</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="5"/>
+        <v>21.85</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="6"/>
+        <v>0.47712125471966244</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="7"/>
+        <v>1.3394514413064407</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="8"/>
+        <v>1.0986122886681098</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="9"/>
+        <v>3.0842009215415991</v>
+      </c>
+      <c r="Y13">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H13" s="11">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="1"/>
         <v>1.0986122886681098</v>
       </c>
-      <c r="I13" s="2">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="K13" s="2">
-        <v>0.255</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="M13" s="2">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="N13" s="2">
-        <v>28.08</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>21.85</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="3"/>
-        <v>21.85</v>
-      </c>
-      <c r="U13">
-        <f>LOG(S13)</f>
-        <v>0.47712125471966244</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="4"/>
-        <v>1.3394514413064407</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="5"/>
-        <v>1.0986122886681098</v>
-      </c>
-      <c r="X13">
-        <f t="shared" si="6"/>
-        <v>3.0842009215415991</v>
-      </c>
-      <c r="Y13">
-        <f>O13</f>
-        <v>0.31900000000000001</v>
-      </c>
-      <c r="Z13">
-        <f>LN(S13)</f>
-        <v>1.0986122886681098</v>
-      </c>
       <c r="AA13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.1425641761972924</v>
       </c>
     </row>
-    <row r="14" spans="6:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="3"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.318</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="M14" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <v>25.89</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P14" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>20.88</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>20.88</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="7"/>
+        <v>1.3197304943302246</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="8"/>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="9"/>
+        <v>3.0387917630144381</v>
+      </c>
+      <c r="Y14">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H14" s="11">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="Z14">
         <f t="shared" si="1"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="I14" s="2">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0.318</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="M14" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="N14" s="2">
-        <v>25.89</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="P14" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>20.88</v>
-      </c>
-      <c r="S14">
+      <c r="AA14">
+        <f t="shared" si="10"/>
+        <v>-1.4188175528254507</v>
+      </c>
+    </row>
+    <row r="15" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="8">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="T14">
+      <c r="H15" s="10">
         <f t="shared" si="3"/>
-        <v>20.88</v>
-      </c>
-      <c r="U14">
-        <f>LOG(S14)</f>
+        <v>0.69314718055994529</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.432</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="N15" s="2">
+        <v>32.56</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="P15" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>27.3</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="5"/>
+        <v>27.3</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="6"/>
         <v>0.3010299956639812</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="4"/>
-        <v>1.3197304943302246</v>
-      </c>
-      <c r="W14">
-        <f t="shared" si="5"/>
+      <c r="V15">
+        <f t="shared" si="7"/>
+        <v>1.436162647040756</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="8"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="X14">
-        <f t="shared" si="6"/>
-        <v>3.0387917630144381</v>
-      </c>
-      <c r="Y14">
-        <f>O14</f>
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="Z14">
-        <f>LN(S14)</f>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="7"/>
-        <v>-1.4188175528254507</v>
-      </c>
-    </row>
-    <row r="15" spans="6:27" ht="30" x14ac:dyDescent="0.25">
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="X15">
+        <f t="shared" si="9"/>
+        <v>3.3068867021909143</v>
+      </c>
+      <c r="Y15">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H15" s="11">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="Z15">
         <f t="shared" si="1"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="I15" s="2">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.432</v>
-      </c>
-      <c r="K15" s="2">
-        <v>0.36599999999999999</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="N15" s="2">
-        <v>32.56</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>27.3</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="T15">
-        <f t="shared" si="3"/>
-        <v>27.3</v>
-      </c>
-      <c r="U15">
-        <f>LOG(S15)</f>
-        <v>0.3010299956639812</v>
-      </c>
-      <c r="V15">
-        <f t="shared" si="4"/>
-        <v>1.436162647040756</v>
-      </c>
-      <c r="W15">
-        <f t="shared" si="5"/>
-        <v>0.69314718055994529</v>
-      </c>
-      <c r="X15">
-        <f t="shared" si="6"/>
-        <v>3.3068867021909143</v>
-      </c>
-      <c r="Y15">
-        <f>O15</f>
-        <v>0.17699999999999999</v>
-      </c>
-      <c r="Z15">
-        <f>LN(S15)</f>
-        <v>0.69314718055994529</v>
-      </c>
       <c r="AA15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.731605546408308</v>
       </c>
     </row>
-    <row r="16" spans="6:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="3"/>
+        <v>0.18232155679395459</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.109</v>
+      </c>
+      <c r="N16" s="2">
+        <v>29.17</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.223</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>23.9</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>23.9</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>7.9181246047624818E-2</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="7"/>
+        <v>1.3783979009481377</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="8"/>
+        <v>0.18232155679395459</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="9"/>
+        <v>3.1738784589374651</v>
+      </c>
+      <c r="Y16">
         <f t="shared" si="0"/>
-        <v>1.2</v>
-      </c>
-      <c r="H16" s="11">
+        <v>0.223</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="1"/>
         <v>0.18232155679395459</v>
       </c>
-      <c r="I16" s="2">
-        <v>0.43</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.32100000000000001</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="L16" s="2">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="M16" s="2">
-        <v>0.109</v>
-      </c>
-      <c r="N16" s="2">
-        <v>29.17</v>
-      </c>
-      <c r="O16" s="2">
-        <v>0.223</v>
-      </c>
-      <c r="P16" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>23.9</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="2"/>
-        <v>1.2</v>
-      </c>
-      <c r="T16">
-        <f t="shared" si="3"/>
-        <v>23.9</v>
-      </c>
-      <c r="U16">
-        <f>LOG(S16)</f>
-        <v>7.9181246047624818E-2</v>
-      </c>
-      <c r="V16">
-        <f t="shared" si="4"/>
-        <v>1.3783979009481377</v>
-      </c>
-      <c r="W16">
-        <f t="shared" si="5"/>
-        <v>0.18232155679395459</v>
-      </c>
-      <c r="X16">
-        <f t="shared" si="6"/>
-        <v>3.1738784589374651</v>
-      </c>
-      <c r="Y16">
-        <f>O16</f>
-        <v>0.223</v>
-      </c>
-      <c r="Z16">
-        <f>LN(S16)</f>
-        <v>0.18232155679395459</v>
-      </c>
       <c r="AA16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.5005835075220182</v>
       </c>
     </row>
-    <row r="17" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M17" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <v>34.19</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>29.22</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="5"/>
+        <v>29.22</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="7"/>
+        <v>1.4656802115982779</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="9"/>
+        <v>3.3748534063225533</v>
+      </c>
+      <c r="Y17">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H17" s="11">
+        <v>0.15</v>
+      </c>
+      <c r="Z17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I17" s="2">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.42299999999999999</v>
-      </c>
-      <c r="K17" s="2">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="M17" s="2">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="N17" s="2">
-        <v>34.19</v>
-      </c>
-      <c r="O17" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="P17" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="Q17" s="2">
-        <v>29.22</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="T17">
-        <f t="shared" si="3"/>
-        <v>29.22</v>
-      </c>
-      <c r="U17">
-        <f>LOG(S17)</f>
-        <v>0</v>
-      </c>
-      <c r="V17">
-        <f t="shared" si="4"/>
-        <v>1.4656802115982779</v>
-      </c>
-      <c r="W17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X17">
-        <f t="shared" si="6"/>
-        <v>3.3748534063225533</v>
-      </c>
-      <c r="Y17">
-        <f>O17</f>
-        <v>0.15</v>
-      </c>
-      <c r="Z17">
-        <f>LN(S17)</f>
-        <v>0</v>
-      </c>
       <c r="AA17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.8971199848858813</v>
       </c>
     </row>
-    <row r="18" spans="6:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:27" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="H18" s="11">
+        <f t="shared" si="3"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="N18" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>31.63</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="5"/>
+        <v>31.63</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="6"/>
+        <v>-0.22184874961635639</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="7"/>
+        <v>1.5000991919157229</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="8"/>
+        <v>-0.51082562376599072</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="9"/>
+        <v>3.4541060373175574</v>
+      </c>
+      <c r="Y18">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="H18" s="12">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="Z18">
         <f t="shared" si="1"/>
         <v>-0.51082562376599072</v>
       </c>
-      <c r="I18" s="2">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="K18" s="2">
-        <v>0.39600000000000002</v>
-      </c>
-      <c r="L18" s="2">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="M18" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="N18" s="2">
-        <v>37.299999999999997</v>
-      </c>
-      <c r="O18" s="2">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>31.63</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="3"/>
-        <v>31.63</v>
-      </c>
-      <c r="U18">
-        <f>LOG(S18)</f>
-        <v>-0.22184874961635639</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="4"/>
-        <v>1.5000991919157229</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="5"/>
-        <v>-0.51082562376599072</v>
-      </c>
-      <c r="X18">
-        <f t="shared" si="6"/>
-        <v>3.4541060373175574</v>
-      </c>
-      <c r="Y18">
-        <f>O18</f>
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="Z18">
-        <f>LN(S18)</f>
-        <v>-0.51082562376599072</v>
-      </c>
       <c r="AA18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>-1.8018098050815563</v>
       </c>
     </row>
@@ -11400,20 +11400,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11436,6 +11436,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2FDDBA-8E4A-41B0-9357-134C9F5B7B79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -11450,12 +11458,4 @@
     <ds:schemaRef ds:uri="c2fb78ee-7f80-47d5-98b2-7e891369b7bb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
// store before branch soil moisture
</commit_message>
<xml_diff>
--- a/auxfiles/GSSHApedotransfer.xlsx
+++ b/auxfiles/GSSHApedotransfer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisemgit\openlisem\auxfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC4FE7D-B358-43EF-BA8F-3D0F31B8F58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE2F88C-1CCB-414C-8123-D1CE6FBDB79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{EE7E3014-B43F-4E75-BCA9-657834F4F7BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>Sand</t>
   </si>
@@ -311,12 +311,6 @@
     </r>
   </si>
   <si>
-    <t>lnks</t>
-  </si>
-  <si>
-    <t>lnlog</t>
-  </si>
-  <si>
     <t>ks (mm/h)</t>
   </si>
   <si>
@@ -324,6 +318,18 @@
   </si>
   <si>
     <t>ln(ks)</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>ln(lambda)</t>
+  </si>
+  <si>
+    <t>ln(psi)</t>
+  </si>
+  <si>
+    <t>ln(bub)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +695,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$8:$Y$18</c:f>
+              <c:f>Sheet1!$Z$8:$Z$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -869,6 +875,434 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1958512127"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="nl-NL"/>
+              <a:t>ln(bub) = ln(ks)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-9.5097331583552061E-2"/>
+                  <c:y val="0.11358267716535433"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="nl-NL"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$AA$8:$AA$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.4621354517774314</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0910056609565864</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0819099697950434</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5802168295923251</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9169226121820611</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0986122886681098</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69314718055994529</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69314718055994529</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18232155679395459</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.51082562376599072</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$AC$8:$AC$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.9823798288367047</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1621729392773008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6851226964585053</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.411439497906128</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0344721018699214</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3350575791576103</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.2538567937634464</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.4830845411343394</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.3731407838796299</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5319332036512097</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.6189933266497696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C89F-4724-8285-2B34186920FD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1774120032"/>
+        <c:axId val="1774120512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1774120032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1774120512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1774120512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1774120032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1455,7 +1889,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$Z$8:$Z$18</c:f>
+              <c:f>Sheet1!$AA$8:$AA$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1497,7 +1931,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AA$8:$AA$18</c:f>
+              <c:f>Sheet1!$AB$8:$AB$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2300,7 +2734,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$U$8:$U$18</c:f>
+              <c:f>Sheet1!$V$8:$V$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2342,7 +2776,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$V$8:$V$18</c:f>
+              <c:f>Sheet1!$W$8:$W$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2855,7 +3289,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$W$8:$W$18</c:f>
+              <c:f>Sheet1!$X$8:$X$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2897,7 +3331,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$X$8:$X$18</c:f>
+              <c:f>Sheet1!$Y$8:$Y$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3146,409 +3580,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="nl-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="power"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-7.5754593175853015E-3"/>
-                  <c:y val="-0.35628244386118402"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="nl-NL"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$S$8:$S$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>235.6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>59.800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.200000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.8000000000000007</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$T$8:$T$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>4.95</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.13</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.89</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.68</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>21.85</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>20.88</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>27.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>23.9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>29.22</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>31.63</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E4BC-489B-90F9-522EB361F2D0}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="293478560"/>
-        <c:axId val="293480000"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="293478560"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="293480000"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="293480000"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nl-NL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="293478560"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="nl-NL"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -3970,7 +4001,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4408,7 +4439,400 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nl-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$V$8:$V$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>2.372175286115064</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7767011839884108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3384564936046048</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1205739312058498</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83250891270623639</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.47712125471966244</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9181246047624818E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.22184874961635639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$W$8:$W$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.69460519893356876</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78746047451841505</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0417873189717517</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94890176097021373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2221960463017199</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3394514413064407</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3197304943302246</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.436162647040756</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3783979009481377</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4656802115982779</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5000991919157229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8331-49F5-A594-6D38762ADE35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2130082832"/>
+        <c:axId val="2130070832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2130082832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2130070832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2130070832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2130082832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -5284,6 +5708,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9540,13 +10480,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
+      <xdr:col>40</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>233362</xdr:rowOff>
@@ -9576,16 +10516,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>33336</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>319087</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>353376</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>60007</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>15239</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9612,13 +10552,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>23812</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>328612</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>204787</xdr:rowOff>
@@ -9648,13 +10588,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>74295</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>50482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>379095</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>75247</xdr:rowOff>
@@ -9684,16 +10624,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>361951</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>125731</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>466726</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>230506</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>26670</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9720,16 +10660,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>530543</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>8571</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50483</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>107631</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>225743</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>77151</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>355283</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9756,23 +10696,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>426243</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>164306</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>100489</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>26193</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>121443</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>50006</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>205264</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>102393</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 10">
+        <xdr:cNvPr id="13" name="Chart 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F057B42C-4C6B-642B-53E5-0EC100090672}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99845C40-37C8-0533-C7FF-EB8CDBB07476}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9792,23 +10732,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>54769</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>102393</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>233841</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>115253</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>159544</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>178593</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>538641</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>16193</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12">
+        <xdr:cNvPr id="14" name="Chart 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99845C40-37C8-0533-C7FF-EB8CDBB07476}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E300D210-8F67-8B4E-5F29-08AD93865A4A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9828,23 +10768,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584361</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>267653</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>279561</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>168593</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="14" name="Chart 13">
+        <xdr:cNvPr id="15" name="Chart 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E300D210-8F67-8B4E-5F29-08AD93865A4A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12A3BE07-F3ED-414B-408D-BD5E19A4B07E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9857,6 +10797,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73326B74-A495-F410-0360-1CA73250708F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10162,10 +11138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC7A993-96B8-4AA6-8EF4-C236C394CA84}">
-  <dimension ref="F1:AA18"/>
+  <dimension ref="F1:AC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J6" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10173,26 +11149,26 @@
     <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F1" s="4" t="s">
         <v>34</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="3" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="6:27" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="6:29" ht="129.6" x14ac:dyDescent="0.3">
       <c r="F4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
@@ -10223,7 +11199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="6:27" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="F5" s="12"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -10255,7 +11231,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="6:27" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="6:29" ht="45" x14ac:dyDescent="0.3">
       <c r="F6" s="12"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -10292,25 +11268,38 @@
       <c r="T6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="U6" s="2"/>
+      <c r="V6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="W6" s="2" t="s">
+      <c r="X6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="6:29" x14ac:dyDescent="0.3">
+      <c r="G7" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="6:27" x14ac:dyDescent="0.3">
-      <c r="G7" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="H7" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="S7" t="s">
         <v>36</v>
@@ -10319,7 +11308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
@@ -10366,36 +11355,40 @@
         <f>Q8</f>
         <v>4.95</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <f>LOG(S8)</f>
         <v>2.372175286115064</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <f>LOG(T8)</f>
         <v>0.69460519893356876</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f>LN(S8)</f>
         <v>5.4621354517774314</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f>LN(T8)</f>
         <v>1.5993875765805989</v>
       </c>
-      <c r="Y8">
-        <f t="shared" ref="Y8:Y18" si="0">O8</f>
+      <c r="Z8">
+        <f t="shared" ref="Z8:Z18" si="0">O8</f>
         <v>0.69399999999999995</v>
       </c>
-      <c r="Z8">
-        <f t="shared" ref="Z8:Z18" si="1">LN(S8)</f>
+      <c r="AA8">
+        <f t="shared" ref="AA8:AA18" si="1">LN(S8)</f>
         <v>5.4621354517774314</v>
       </c>
-      <c r="AA8">
-        <f>LN(Y8)</f>
+      <c r="AB8">
+        <f>LN(Z8)</f>
         <v>-0.36528331847533263</v>
       </c>
+      <c r="AC8">
+        <f>LN(N8)</f>
+        <v>1.9823798288367047</v>
+      </c>
     </row>
-    <row r="9" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>1</v>
       </c>
@@ -10442,36 +11435,40 @@
         <f t="shared" ref="T9:T18" si="5">Q9</f>
         <v>6.13</v>
       </c>
-      <c r="U9">
-        <f t="shared" ref="U9:U18" si="6">LOG(S9)</f>
+      <c r="V9">
+        <f t="shared" ref="V9:V18" si="6">LOG(S9)</f>
         <v>1.7767011839884108</v>
       </c>
-      <c r="V9">
-        <f t="shared" ref="V9:V18" si="7">LOG(T9)</f>
+      <c r="W9">
+        <f t="shared" ref="W9:W18" si="7">LOG(T9)</f>
         <v>0.78746047451841505</v>
       </c>
-      <c r="W9">
-        <f t="shared" ref="W9:W18" si="8">LN(S9)</f>
+      <c r="X9">
+        <f t="shared" ref="X9:X18" si="8">LN(S9)</f>
         <v>4.0910056609565864</v>
       </c>
-      <c r="X9">
-        <f t="shared" ref="X9:X18" si="9">LN(T9)</f>
+      <c r="Y9">
+        <f t="shared" ref="Y9:Y18" si="9">LN(T9)</f>
         <v>1.81319474994812</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <f t="shared" si="0"/>
         <v>0.55300000000000005</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <f t="shared" si="1"/>
         <v>4.0910056609565864</v>
       </c>
-      <c r="AA9">
-        <f t="shared" ref="AA9:AA18" si="10">LN(Y9)</f>
+      <c r="AB9">
+        <f t="shared" ref="AB9:AB18" si="10">LN(Z9)</f>
         <v>-0.5923972774598022</v>
       </c>
+      <c r="AC9">
+        <f t="shared" ref="AC9:AC18" si="11">LN(N9)</f>
+        <v>2.1621729392773008</v>
+      </c>
     </row>
-    <row r="10" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>2</v>
       </c>
@@ -10518,36 +11515,40 @@
         <f t="shared" si="5"/>
         <v>11.01</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <f t="shared" si="6"/>
         <v>1.3384564936046048</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <f t="shared" si="7"/>
         <v>1.0417873189717517</v>
       </c>
-      <c r="W10">
+      <c r="X10">
         <f t="shared" si="8"/>
         <v>3.0819099697950434</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <f t="shared" si="9"/>
         <v>2.3988039507345884</v>
       </c>
-      <c r="Y10">
+      <c r="Z10">
         <f t="shared" si="0"/>
         <v>0.378</v>
       </c>
-      <c r="Z10">
+      <c r="AA10">
         <f t="shared" si="1"/>
         <v>3.0819099697950434</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <f t="shared" si="10"/>
         <v>-0.97286108336254939</v>
       </c>
+      <c r="AC10">
+        <f t="shared" si="11"/>
+        <v>2.6851226964585053</v>
+      </c>
     </row>
-    <row r="11" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F11" s="1" t="s">
         <v>3</v>
       </c>
@@ -10594,36 +11595,40 @@
         <f t="shared" si="5"/>
         <v>8.89</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <f t="shared" si="6"/>
         <v>1.1205739312058498</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <f t="shared" si="7"/>
         <v>0.94890176097021373</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <f t="shared" si="8"/>
         <v>2.5802168295923251</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f t="shared" si="9"/>
         <v>2.1849270495258133</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <f t="shared" si="0"/>
         <v>0.252</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <f t="shared" si="1"/>
         <v>2.5802168295923251</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <f t="shared" si="10"/>
         <v>-1.3783261914707137</v>
       </c>
+      <c r="AC11">
+        <f t="shared" si="11"/>
+        <v>2.411439497906128</v>
+      </c>
     </row>
-    <row r="12" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
@@ -10670,36 +11675,40 @@
         <f t="shared" si="5"/>
         <v>16.68</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <f t="shared" si="6"/>
         <v>0.83250891270623639</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <f t="shared" si="7"/>
         <v>1.2221960463017199</v>
       </c>
-      <c r="W12">
+      <c r="X12">
         <f t="shared" si="8"/>
         <v>1.9169226121820611</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <f t="shared" si="9"/>
         <v>2.8142103969306005</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <f t="shared" si="0"/>
         <v>0.23400000000000001</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <f t="shared" si="1"/>
         <v>1.9169226121820611</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <f t="shared" si="10"/>
         <v>-1.4524341636244356</v>
       </c>
+      <c r="AC12">
+        <f t="shared" si="11"/>
+        <v>3.0344721018699214</v>
+      </c>
     </row>
-    <row r="13" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F13" s="1" t="s">
         <v>5</v>
       </c>
@@ -10746,36 +11755,40 @@
         <f t="shared" si="5"/>
         <v>21.85</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <f t="shared" si="6"/>
         <v>0.47712125471966244</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <f t="shared" si="7"/>
         <v>1.3394514413064407</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <f t="shared" si="8"/>
         <v>1.0986122886681098</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <f t="shared" si="9"/>
         <v>3.0842009215415991</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <f t="shared" si="0"/>
         <v>0.31900000000000001</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <f t="shared" si="1"/>
         <v>1.0986122886681098</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <f t="shared" si="10"/>
         <v>-1.1425641761972924</v>
       </c>
+      <c r="AC13">
+        <f t="shared" si="11"/>
+        <v>3.3350575791576103</v>
+      </c>
     </row>
-    <row r="14" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F14" s="1" t="s">
         <v>6</v>
       </c>
@@ -10822,36 +11835,40 @@
         <f t="shared" si="5"/>
         <v>20.88</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <f t="shared" si="6"/>
         <v>0.3010299956639812</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <f t="shared" si="7"/>
         <v>1.3197304943302246</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <f t="shared" si="8"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <f t="shared" si="9"/>
         <v>3.0387917630144381</v>
       </c>
-      <c r="Y14">
+      <c r="Z14">
         <f t="shared" si="0"/>
         <v>0.24199999999999999</v>
       </c>
-      <c r="Z14">
+      <c r="AA14">
         <f t="shared" si="1"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <f t="shared" si="10"/>
         <v>-1.4188175528254507</v>
       </c>
+      <c r="AC14">
+        <f t="shared" si="11"/>
+        <v>3.2538567937634464</v>
+      </c>
     </row>
-    <row r="15" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F15" s="1" t="s">
         <v>7</v>
       </c>
@@ -10898,36 +11915,40 @@
         <f t="shared" si="5"/>
         <v>27.3</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <f t="shared" si="6"/>
         <v>0.3010299956639812</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <f t="shared" si="7"/>
         <v>1.436162647040756</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <f t="shared" si="8"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <f t="shared" si="9"/>
         <v>3.3068867021909143</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <f t="shared" si="0"/>
         <v>0.17699999999999999</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <f t="shared" si="1"/>
         <v>0.69314718055994529</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <f t="shared" si="10"/>
         <v>-1.731605546408308</v>
       </c>
+      <c r="AC15">
+        <f t="shared" si="11"/>
+        <v>3.4830845411343394</v>
+      </c>
     </row>
-    <row r="16" spans="6:27" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:29" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F16" s="1" t="s">
         <v>8</v>
       </c>
@@ -10974,36 +11995,40 @@
         <f t="shared" si="5"/>
         <v>23.9</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <f t="shared" si="6"/>
         <v>7.9181246047624818E-2</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <f t="shared" si="7"/>
         <v>1.3783979009481377</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <f t="shared" si="8"/>
         <v>0.18232155679395459</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <f t="shared" si="9"/>
         <v>3.1738784589374651</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <f t="shared" si="0"/>
         <v>0.223</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <f t="shared" si="1"/>
         <v>0.18232155679395459</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <f t="shared" si="10"/>
         <v>-1.5005835075220182</v>
       </c>
+      <c r="AC16">
+        <f t="shared" si="11"/>
+        <v>3.3731407838796299</v>
+      </c>
     </row>
-    <row r="17" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
@@ -11050,36 +12075,40 @@
         <f t="shared" si="5"/>
         <v>29.22</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <f t="shared" si="7"/>
         <v>1.4656802115982779</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <f t="shared" si="9"/>
         <v>3.3748534063225533</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <f t="shared" si="10"/>
         <v>-1.8971199848858813</v>
       </c>
+      <c r="AC17">
+        <f t="shared" si="11"/>
+        <v>3.5319332036512097</v>
+      </c>
     </row>
-    <row r="18" spans="6:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:29" x14ac:dyDescent="0.3">
       <c r="F18" s="1" t="s">
         <v>10</v>
       </c>
@@ -11126,33 +12155,37 @@
         <f t="shared" si="5"/>
         <v>31.63</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <f t="shared" si="6"/>
         <v>-0.22184874961635639</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <f t="shared" si="7"/>
         <v>1.5000991919157229</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <f t="shared" si="8"/>
         <v>-0.51082562376599072</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <f t="shared" si="9"/>
         <v>3.4541060373175574</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <f t="shared" si="0"/>
         <v>0.16500000000000001</v>
       </c>
-      <c r="Z18">
+      <c r="AA18">
         <f t="shared" si="1"/>
         <v>-0.51082562376599072</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <f t="shared" si="10"/>
         <v>-1.8018098050815563</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" si="11"/>
+        <v>3.6189933266497696</v>
       </c>
     </row>
   </sheetData>
@@ -11400,20 +12433,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c2fb78ee-7f80-47d5-98b2-7e891369b7bb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11436,14 +12469,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F2FDDBA-8E4A-41B0-9357-134C9F5B7B79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -11458,4 +12483,12 @@
     <ds:schemaRef ds:uri="c2fb78ee-7f80-47d5-98b2-7e891369b7bb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{546FAC25-7A53-4BE4-87D4-6463C2D97D48}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>